<commit_message>
Se pueden suspender lengua y matemáticas y promocionar
</commit_message>
<xml_diff>
--- a/apuntes/5/ejercicios-excel/enunciados-ejercicios-excel.xlsx
+++ b/apuntes/5/ejercicios-excel/enunciados-ejercicios-excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15180" windowHeight="10110" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15180" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Promoción" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Nombre</t>
   </si>
@@ -68,9 +68,6 @@
     <t>TICO</t>
   </si>
   <si>
-    <t>http://www.mecd.gob.es/educacion-mecd/areas-educacion/estudiantes/bachillerato/informacion-general/evaluacion-promocion.html</t>
-  </si>
-  <si>
     <t>Inglés</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Promociona</t>
   </si>
   <si>
-    <t>Normativa</t>
-  </si>
-  <si>
     <t>Alumno</t>
   </si>
   <si>
@@ -144,12 +138,6 @@
   </si>
   <si>
     <t>Tipo de IVA</t>
-  </si>
-  <si>
-    <t>Completa la hoja excel para calcular automáticamente los alumnos que promocionan a segundo de bachillerato, según la normativa.
-Supondremos que  sólo hay 5 asignaturas.
-La columna PROMOCIONA se rellenará automáticamente a SI o NO según las notas de las asignaturas.
-Cuando la hoja esté acabada, el usuario sólo escribirá en las casillas en azul, el resto se recalculará automáticamente.</t>
   </si>
   <si>
     <t>Los ticket de los supermercados deben incluir desglosado el IVA.
@@ -239,6 +227,12 @@
   </si>
   <si>
     <t>Platos</t>
+  </si>
+  <si>
+    <t>Completa la hoja excel para calcular automáticamente los alumnos que promocionan a segundo de bachillerato, según la normativa.
+Supondremos que  sólo hay 5 asignaturas, y que se pueden suspender cualesquiera dos para poder promocinar.
+La columna PROMOCIONA se rellenará automáticamente a SI o NO según las notas de las asignaturas.
+Cuando la hoja esté acabada, el usuario sólo escribirá en las casillas en azul, el resto se recalculará automáticamente.</t>
   </si>
 </sst>
 </file>
@@ -525,6 +519,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -540,8 +536,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1283,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,41 +1288,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="A2" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="40"/>
+      <c r="A4" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="42"/>
+      <c r="C4" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1348,21 +1337,21 @@
         <v>4</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="12">
         <v>7</v>
@@ -1379,14 +1368,14 @@
       <c r="G6" s="14">
         <v>7</v>
       </c>
-      <c r="H6" s="43"/>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="12">
         <v>7</v>
@@ -1403,14 +1392,14 @@
       <c r="G7" s="14">
         <v>6</v>
       </c>
-      <c r="H7" s="44"/>
+      <c r="H7" s="39"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="12">
         <v>5</v>
@@ -1427,14 +1416,14 @@
       <c r="G8" s="14">
         <v>9</v>
       </c>
-      <c r="H8" s="44"/>
+      <c r="H8" s="39"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="12">
         <v>4</v>
@@ -1451,14 +1440,14 @@
       <c r="G9" s="14">
         <v>6</v>
       </c>
-      <c r="H9" s="44"/>
+      <c r="H9" s="39"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="12">
         <v>6</v>
@@ -1475,14 +1464,14 @@
       <c r="G10" s="14">
         <v>5</v>
       </c>
-      <c r="H10" s="44"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="12">
         <v>4</v>
@@ -1499,14 +1488,14 @@
       <c r="G11" s="14">
         <v>9</v>
       </c>
-      <c r="H11" s="44"/>
+      <c r="H11" s="39"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="12">
         <v>4</v>
@@ -1523,14 +1512,14 @@
       <c r="G12" s="14">
         <v>5</v>
       </c>
-      <c r="H12" s="44"/>
+      <c r="H12" s="39"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="15">
         <v>4</v>
@@ -1561,11 +1550,8 @@
       <formula2>10</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1587,46 +1573,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
       <c r="G1" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D9" s="13">
         <v>1</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F9" s="26">
         <v>10</v>
@@ -1636,13 +1622,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D10" s="13">
         <v>1</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F10" s="26">
         <v>40</v>
@@ -1652,13 +1638,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" s="13">
         <v>1</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F11" s="26">
         <v>300</v>
@@ -1695,7 +1681,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G15" s="32">
         <f>SUM(G9:G14)</f>
@@ -1717,7 +1703,7 @@
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D18" s="28">
         <v>0.21</v>
@@ -1729,7 +1715,7 @@
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D19" s="28">
         <v>0.1</v>
@@ -1741,7 +1727,7 @@
     </row>
     <row r="20" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D20" s="29">
         <v>0.04</v>
@@ -1770,7 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -1785,18 +1771,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C6" s="22">
         <v>100</v>
@@ -1805,7 +1791,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" s="23">
         <v>1.5</v>
@@ -1814,7 +1800,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" s="23">
         <v>3</v>
@@ -1822,7 +1808,7 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="19"/>
       <c r="K9" s="36"/>
@@ -1833,96 +1819,96 @@
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E14" s="20"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E15" s="20"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="20"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E17" s="20"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E18" s="20"/>
     </row>
@@ -1940,7 +1926,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E21" s="37">
         <f>SUM(E12:E20)</f>

</xml_diff>